<commit_message>
Improved ExcelReaderTest and DatafileTest
</commit_message>
<xml_diff>
--- a/input/src/test/resources/website_test2.xlsx
+++ b/input/src/test/resources/website_test2.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26009"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aproj\contextz\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbakker/Contextproject2015/input/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="0" windowWidth="19080" windowHeight="8355"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="19080" windowHeight="8360"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="35">
   <si>
     <t>custommeasurementitem_141214.Id</t>
   </si>
@@ -240,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -324,11 +327,11 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="38004A"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -364,7 +367,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -436,7 +439,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,16 +592,16 @@
   <dimension ref="A1:W58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +665,7 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>726</v>
       </c>
@@ -726,7 +729,7 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>727</v>
       </c>
@@ -790,7 +793,7 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>728</v>
       </c>
@@ -854,7 +857,7 @@
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
     </row>
-    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>729</v>
       </c>
@@ -918,7 +921,7 @@
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
     </row>
-    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>730</v>
       </c>
@@ -946,9 +949,7 @@
       <c r="I6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
@@ -982,7 +983,7 @@
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>731</v>
       </c>
@@ -1046,7 +1047,7 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>732</v>
       </c>
@@ -1110,7 +1111,7 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
     </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>733</v>
       </c>
@@ -1174,7 +1175,7 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
     </row>
-    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>734</v>
       </c>
@@ -1238,7 +1239,7 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
     </row>
-    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>735</v>
       </c>
@@ -1302,7 +1303,7 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
     </row>
-    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>736</v>
       </c>
@@ -1366,7 +1367,7 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
     </row>
-    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>737</v>
       </c>
@@ -1430,7 +1431,7 @@
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
     </row>
-    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>738</v>
       </c>
@@ -1494,7 +1495,7 @@
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
     </row>
-    <row r="15" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>739</v>
       </c>
@@ -1558,7 +1559,7 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
     </row>
-    <row r="16" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>740</v>
       </c>
@@ -1622,7 +1623,7 @@
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
     </row>
-    <row r="17" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>741</v>
       </c>
@@ -1686,7 +1687,7 @@
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
     </row>
-    <row r="18" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>742</v>
       </c>
@@ -1750,7 +1751,7 @@
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
     </row>
-    <row r="19" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>743</v>
       </c>
@@ -1814,7 +1815,7 @@
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
     </row>
-    <row r="20" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>744</v>
       </c>
@@ -1878,7 +1879,7 @@
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
     </row>
-    <row r="21" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>745</v>
       </c>
@@ -1942,7 +1943,7 @@
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
     </row>
-    <row r="22" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>746</v>
       </c>
@@ -2006,7 +2007,7 @@
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
     </row>
-    <row r="23" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>747</v>
       </c>
@@ -2070,7 +2071,7 @@
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
     </row>
-    <row r="24" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>748</v>
       </c>
@@ -2134,7 +2135,7 @@
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
     </row>
-    <row r="25" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>749</v>
       </c>
@@ -2198,7 +2199,7 @@
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
     </row>
-    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>750</v>
       </c>
@@ -2262,7 +2263,7 @@
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
     </row>
-    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>751</v>
       </c>
@@ -2326,7 +2327,7 @@
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
     </row>
-    <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>752</v>
       </c>
@@ -2390,7 +2391,7 @@
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
     </row>
-    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>753</v>
       </c>
@@ -2454,7 +2455,7 @@
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
     </row>
-    <row r="30" spans="1:23" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>754</v>
       </c>
@@ -2518,7 +2519,7 @@
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
     </row>
-    <row r="31" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>755</v>
       </c>
@@ -2582,7 +2583,7 @@
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
     </row>
-    <row r="32" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>756</v>
       </c>
@@ -2646,7 +2647,7 @@
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
     </row>
-    <row r="33" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>757</v>
       </c>
@@ -2710,7 +2711,7 @@
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
     </row>
-    <row r="34" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>758</v>
       </c>
@@ -2774,7 +2775,7 @@
       <c r="V34" s="4"/>
       <c r="W34" s="4"/>
     </row>
-    <row r="35" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>759</v>
       </c>
@@ -2838,7 +2839,7 @@
       <c r="V35" s="4"/>
       <c r="W35" s="4"/>
     </row>
-    <row r="36" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>760</v>
       </c>
@@ -2902,7 +2903,7 @@
       <c r="V36" s="4"/>
       <c r="W36" s="4"/>
     </row>
-    <row r="37" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>761</v>
       </c>
@@ -2966,7 +2967,7 @@
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
     </row>
-    <row r="38" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>762</v>
       </c>
@@ -3027,7 +3028,7 @@
       <c r="V38" s="4"/>
       <c r="W38" s="4"/>
     </row>
-    <row r="39" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>763</v>
       </c>
@@ -3091,7 +3092,7 @@
       <c r="V39" s="4"/>
       <c r="W39" s="4"/>
     </row>
-    <row r="40" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>764</v>
       </c>
@@ -3155,7 +3156,7 @@
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
     </row>
-    <row r="41" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>765</v>
       </c>
@@ -3219,7 +3220,7 @@
       <c r="V41" s="4"/>
       <c r="W41" s="4"/>
     </row>
-    <row r="42" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>766</v>
       </c>
@@ -3280,7 +3281,7 @@
       <c r="V42" s="4"/>
       <c r="W42" s="4"/>
     </row>
-    <row r="43" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>767</v>
       </c>
@@ -3344,7 +3345,7 @@
       <c r="V43" s="4"/>
       <c r="W43" s="4"/>
     </row>
-    <row r="44" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>768</v>
       </c>
@@ -3405,7 +3406,7 @@
       <c r="V44" s="4"/>
       <c r="W44" s="4"/>
     </row>
-    <row r="45" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>769</v>
       </c>
@@ -3469,7 +3470,7 @@
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
     </row>
-    <row r="46" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>770</v>
       </c>
@@ -3533,7 +3534,7 @@
       <c r="V46" s="4"/>
       <c r="W46" s="4"/>
     </row>
-    <row r="47" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>771</v>
       </c>
@@ -3597,7 +3598,7 @@
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
     </row>
-    <row r="48" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>772</v>
       </c>
@@ -3661,7 +3662,7 @@
       <c r="V48" s="4"/>
       <c r="W48" s="4"/>
     </row>
-    <row r="49" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>773</v>
       </c>
@@ -3722,7 +3723,7 @@
       <c r="V49" s="4"/>
       <c r="W49" s="4"/>
     </row>
-    <row r="50" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>774</v>
       </c>
@@ -3786,7 +3787,7 @@
       <c r="V50" s="4"/>
       <c r="W50" s="4"/>
     </row>
-    <row r="51" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>775</v>
       </c>
@@ -3847,7 +3848,7 @@
       <c r="V51" s="4"/>
       <c r="W51" s="4"/>
     </row>
-    <row r="52" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>776</v>
       </c>
@@ -3911,7 +3912,7 @@
       <c r="V52" s="4"/>
       <c r="W52" s="4"/>
     </row>
-    <row r="53" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>777</v>
       </c>
@@ -3972,7 +3973,7 @@
       <c r="V53" s="4"/>
       <c r="W53" s="4"/>
     </row>
-    <row r="54" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>778</v>
       </c>
@@ -4036,7 +4037,7 @@
       <c r="V54" s="4"/>
       <c r="W54" s="4"/>
     </row>
-    <row r="55" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>779</v>
       </c>
@@ -4100,7 +4101,7 @@
       <c r="V55" s="4"/>
       <c r="W55" s="4"/>
     </row>
-    <row r="56" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>780</v>
       </c>
@@ -4164,7 +4165,7 @@
       <c r="V56" s="4"/>
       <c r="W56" s="4"/>
     </row>
-    <row r="57" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>781</v>
       </c>
@@ -4225,7 +4226,7 @@
       <c r="V57" s="4"/>
       <c r="W57" s="4"/>
     </row>
-    <row r="58" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>782</v>
       </c>

</xml_diff>